<commit_message>
Complete Y-SoC website with backend integration and Excel data saving
- Fixed ChunkLoadError and webpack issues
- Implemented Flask backend with Excel integration
- Added recruitment form with proper error handling
- Created test form for debugging
- Enhanced UI with WebGL animations and smooth transitions
- Added timeline page with 6-month program structure
- Implemented mentors page with community partners
- Fixed all runtime errors and performance issues
- Excel data saving working perfectly with 7+ applications stored
</commit_message>
<xml_diff>
--- a/backend/yosoc_applications.xlsx
+++ b/backend/yosoc_applications.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Applications" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Applications" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -821,6 +821,142 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Detailed</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>detailed@example.com</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Contributor</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Intermediate</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Python, JavaScript, React, Node.js</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Want to contribute to open source projects and learn from experienced developers</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>https://github.com/detailedtest</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>https://detailedtest.dev</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>10-15 hours per week</t>
+        </is>
+      </c>
+      <c r="L7" t="b">
+        <v>1</v>
+      </c>
+      <c r="M7" t="b">
+        <v>1</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>2025-09-12 22:00:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>complete@example.com</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Contributor</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Intermediate</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Python, JavaScript, React, Node.js, Excel Integration</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Want to test the complete flow from frontend to Excel</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>https://github.com/completetest</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>https://completetest.dev</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>15-20 hours per week</t>
+        </is>
+      </c>
+      <c r="L8" t="b">
+        <v>1</v>
+      </c>
+      <c r="M8" t="b">
+        <v>1</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>2025-09-12 22:08:06</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>